<commit_message>
New data and added graphs
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DCD42E8-0957-406F-88A4-93C576B1B562}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EAC55CE-51EC-4C47-9BA3-499194584FDF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -8892,6 +8892,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K24" totalsRowShown="0">
   <autoFilter ref="A5:K24" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
@@ -9231,8 +9235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9279,31 +9283,31 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(B6:B55)</f>
+        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B55)</f>
         <v>74.089473684210517</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(C6:C55)</f>
+        <f t="shared" si="0"/>
         <v>10.268421052631579</v>
       </c>
       <c r="D2" s="2">
-        <f>AVERAGE(D6:D55)</f>
-        <v>9.0916666666666668</v>
+        <f t="shared" si="0"/>
+        <v>8.75</v>
       </c>
       <c r="E2" s="2">
-        <f>AVERAGE(E6:E55)</f>
+        <f t="shared" si="0"/>
         <v>14.238888888888889</v>
       </c>
       <c r="F2" s="2">
-        <f>AVERAGE(F6:F55)</f>
+        <f t="shared" si="0"/>
         <v>10.299999999999999</v>
       </c>
       <c r="G2" s="2">
-        <f>AVERAGE(G6:G55)</f>
+        <f t="shared" si="0"/>
         <v>14.100000000000001</v>
       </c>
       <c r="H2" s="2">
-        <f>AVERAGE(H6:H55)</f>
+        <f t="shared" si="0"/>
         <v>8.8666666666666654</v>
       </c>
     </row>
@@ -9316,27 +9320,27 @@
         <v>75.599999999999994</v>
       </c>
       <c r="C3">
-        <f>MIN(C6:C62)</f>
+        <f t="shared" ref="C3:H3" si="1">MIN(C6:C62)</f>
         <v>5.4</v>
       </c>
       <c r="D3">
-        <f>MIN(D6:D62)</f>
+        <f t="shared" si="1"/>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f>MIN(E6:E62)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F3">
-        <f>MIN(F6:F62)</f>
+        <f t="shared" si="1"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="G3">
-        <f>MIN(G6:G62)</f>
+        <f t="shared" si="1"/>
         <v>7.9</v>
       </c>
       <c r="H3">
-        <f>MIN(H6:H62)</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
     </row>
@@ -9893,7 +9897,9 @@
       <c r="C24">
         <v>7.5</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="52" spans="30:30" x14ac:dyDescent="0.3">
       <c r="AD52" t="s">

</xml_diff>

<commit_message>
Added data and start with new 7day graphs
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CF30E85-D4A2-42F4-9B67-74FBD63EAF48}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{979EEDF4-DDFF-49A4-B741-D5D10E2F16D2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -977,6 +977,9 @@
                 <c:pt idx="18">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1145,6 +1148,9 @@
                 <c:pt idx="18">
                   <c:v>8.4</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1300,6 +1306,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1568,9 +1577,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.9247594050743655E-2"/>
-          <c:y val="0.12541666666666668"/>
+          <c:y val="0.14909185982782341"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.75066817579456024"/>
+          <c:h val="0.72699309876851603"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2168,6 +2177,9 @@
                 <c:pt idx="18">
                   <c:v>9.8000000000000007</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2404,9 +2416,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.6469816272965873E-2"/>
-          <c:y val="0.13004629629629633"/>
+          <c:y val="0.13834445466465026"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.76807255889130344"/>
+          <c:h val="0.75646067364363345"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2584,6 +2596,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2845,9 +2860,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.6933029157768886E-2"/>
-          <c:y val="0.11890665929996908"/>
+          <c:y val="0.15345964025110234"/>
           <c:w val="0.90288133458109276"/>
-          <c:h val="0.77600505276632792"/>
+          <c:h val="0.74145201866761945"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3881,9 +3896,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.6469816272965873E-2"/>
-          <c:y val="0.13004629629629633"/>
+          <c:y val="0.15901680255526221"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.7629246864975211"/>
+          <c:h val="0.7339539908635051"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4052,6 +4067,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8684,7 +8702,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>439269</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>62754</xdr:rowOff>
+      <xdr:rowOff>8965</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8750,13 +8768,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>396240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>14790</xdr:rowOff>
+      <xdr:rowOff>14791</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>80682</xdr:rowOff>
+      <xdr:rowOff>8966</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8786,7 +8804,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>412375</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>80683</xdr:rowOff>
+      <xdr:rowOff>17930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
@@ -8864,7 +8882,7 @@
       <xdr:col>36</xdr:col>
       <xdr:colOff>331694</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>107577</xdr:rowOff>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8892,15 +8910,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>121021</xdr:colOff>
+      <xdr:colOff>138950</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:rowOff>8966</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>385482</xdr:colOff>
+      <xdr:colOff>403411</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>116540</xdr:rowOff>
+      <xdr:rowOff>98611</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9303,8 +9321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL23" sqref="AL23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9351,32 +9369,32 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(B6:B56)</f>
+        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B56)</f>
         <v>74.16</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(C6:C56)</f>
+        <f t="shared" si="0"/>
         <v>10.095000000000001</v>
       </c>
       <c r="D2" s="2">
-        <f>AVERAGE(D6:D56)</f>
-        <v>8.75</v>
+        <f t="shared" si="0"/>
+        <v>8.4937500000000004</v>
       </c>
       <c r="E2" s="2">
-        <f>AVERAGE(E6:E56)</f>
-        <v>14.005263157894738</v>
+        <f t="shared" si="0"/>
+        <v>13.725</v>
       </c>
       <c r="F2" s="2">
-        <f>AVERAGE(F6:F56)</f>
-        <v>10.185714285714285</v>
+        <f t="shared" si="0"/>
+        <v>10.225</v>
       </c>
       <c r="G2" s="2">
-        <f>AVERAGE(G6:G56)</f>
-        <v>13.800000000000002</v>
+        <f t="shared" si="0"/>
+        <v>13.560000000000002</v>
       </c>
       <c r="H2" s="2">
-        <f>AVERAGE(H6:H56)</f>
-        <v>8.8666666666666654</v>
+        <f t="shared" si="0"/>
+        <v>8.6374999999999975</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -9388,28 +9406,28 @@
         <v>75.599999999999994</v>
       </c>
       <c r="C3">
-        <f>MIN(C6:C63)</f>
+        <f t="shared" ref="C3:H3" si="1">MIN(C6:C63)</f>
         <v>5.4</v>
       </c>
       <c r="D3">
-        <f>MIN(D6:D63)</f>
+        <f t="shared" si="1"/>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f>MIN(E6:E63)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F3">
-        <f>MIN(F6:F63)</f>
+        <f t="shared" si="1"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="G3">
-        <f>MIN(G6:G63)</f>
+        <f t="shared" si="1"/>
         <v>7.9</v>
       </c>
       <c r="H3">
-        <f>MIN(H6:H63)</f>
-        <v>5.5</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -9977,6 +9995,9 @@
       <c r="G24">
         <v>8.4</v>
       </c>
+      <c r="H24">
+        <v>5.2</v>
+      </c>
       <c r="I24">
         <v>8</v>
       </c>
@@ -9997,7 +10018,18 @@
       <c r="C25">
         <v>6.8</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="E25">
+        <v>8.4</v>
+      </c>
+      <c r="F25">
+        <v>10.5</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
       <c r="I25">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added data and prepping new graphs
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{979EEDF4-DDFF-49A4-B741-D5D10E2F16D2}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F8EB25D-34D8-4DF7-8A08-92ADBB60380F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -247,10 +247,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -310,16 +310,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$B$6:$B$25</c:f>
+              <c:f>main!$B$6:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>72.400000000000006</c:v>
                 </c:pt>
@@ -379,6 +382,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,10 +682,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -739,16 +745,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$25</c:f>
+              <c:f>main!$C$6:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -808,6 +817,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,10 +859,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -910,16 +922,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$25</c:f>
+              <c:f>main!$E$6:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1018,10 +1033,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1081,16 +1096,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$25</c:f>
+              <c:f>main!$G$6:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -1189,10 +1207,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1252,16 +1270,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$25</c:f>
+              <c:f>main!$H$6:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -1309,6 +1330,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1628,10 +1652,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1691,16 +1715,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$25</c:f>
+              <c:f>main!$C$6:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -1760,6 +1787,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2047,10 +2077,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2110,16 +2140,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$25</c:f>
+              <c:f>main!$E$6:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -2467,10 +2500,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2530,16 +2563,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$25</c:f>
+              <c:f>main!$G$6:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -2914,10 +2950,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2977,16 +3013,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$I$6:$I$25</c:f>
+              <c:f>main!$I$6:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
@@ -3009,6 +3048,9 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3070,10 +3112,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3133,16 +3175,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$J$6:$J$25</c:f>
+              <c:f>main!$J$6:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3201,6 +3246,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3536,10 +3584,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3599,16 +3647,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$K$6:$K$25</c:f>
+              <c:f>main!$K$6:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3658,6 +3709,9 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -3950,10 +4004,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$25</c:f>
+              <c:f>main!$A$6:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4013,16 +4067,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$25</c:f>
+              <c:f>main!$H$6:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -4070,6 +4127,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8983,8 +9043,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K25" totalsRowShown="0">
-  <autoFilter ref="A5:K25" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K26" totalsRowShown="0">
+  <autoFilter ref="A5:K26" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight"/>
@@ -9322,7 +9382,7 @@
   <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9369,32 +9429,32 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B56)</f>
-        <v>74.16</v>
+        <f>AVERAGE(B6:B57)</f>
+        <v>74.238095238095227</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" si="0"/>
-        <v>10.095000000000001</v>
+        <f>AVERAGE(C6:C57)</f>
+        <v>9.8714285714285719</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6:D57)</f>
         <v>8.4937500000000004</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E6:E57)</f>
         <v>13.725</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F6:F57)</f>
         <v>10.225</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G6:G57)</f>
         <v>13.560000000000002</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" si="0"/>
-        <v>8.6374999999999975</v>
+        <f>AVERAGE(H6:H57)</f>
+        <v>8.470588235294116</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -9402,31 +9462,31 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f>MAX(B6:B63)</f>
-        <v>75.599999999999994</v>
+        <f>MAX(B6:B64)</f>
+        <v>75.8</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H3" si="1">MIN(C6:C63)</f>
+        <f>MIN(C6:C64)</f>
         <v>5.4</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
+        <f>MIN(D6:D64)</f>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f>MIN(E6:E64)</f>
         <v>7</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f>MIN(F6:F64)</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>MIN(G6:G64)</f>
         <v>7.9</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
+        <f>MIN(H6:H64)</f>
         <v>5.2</v>
       </c>
     </row>
@@ -10030,10 +10090,34 @@
       <c r="G25">
         <v>9</v>
       </c>
+      <c r="H25">
+        <v>5.8</v>
+      </c>
       <c r="I25">
         <v>10</v>
       </c>
       <c r="J25">
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45483</v>
+      </c>
+      <c r="B26">
+        <v>75.8</v>
+      </c>
+      <c r="C26">
+        <v>5.4</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New data and changed layout with new boxplots and strip charts
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4254522A-189E-4E4C-AE79-5F0EAA73DB0A}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11D2C6C0-0C7C-493D-85D7-64FDE7DD5A15}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Weight</t>
   </si>
@@ -1292,6 +1292,9 @@
                 <c:pt idx="24">
                   <c:v>7.5</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1486,6 +1489,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2881,6 +2887,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4496,6 +4505,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9408,10 +9420,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K31" totalsRowShown="0">
   <autoFilter ref="A5:K31" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
@@ -9752,7 +9760,7 @@
   <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL20" sqref="AL20"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9816,15 +9824,15 @@
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>9.3384615384615373</v>
+        <v>9.1928571428571413</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>12.187999999999999</v>
+        <v>11.923076923076923</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>8.0590909090909086</v>
+        <v>8.0260869565217394</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -10664,11 +10672,25 @@
       <c r="E31">
         <v>7.4</v>
       </c>
+      <c r="F31">
+        <v>7.3</v>
+      </c>
+      <c r="G31">
+        <v>5.3</v>
+      </c>
+      <c r="H31">
+        <v>7.3</v>
+      </c>
       <c r="I31">
         <v>10</v>
       </c>
       <c r="J31">
         <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="30:30" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added data, minor fixes to graphs.
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4791BD40-D73F-4FD1-AAE9-D6955634340F}"/>
+  <xr:revisionPtr revIDLastSave="481" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{148FC3D7-42E6-47AC-B118-53F3340CD415}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
+    <workbookView xWindow="28680" yWindow="-6480" windowWidth="29040" windowHeight="16440" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -124,7 +124,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
     </dxf>
@@ -247,10 +250,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -331,16 +334,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$B$6:$B$32</c:f>
+              <c:f>main!$B$6:$B$33</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>72.400000000000006</c:v>
                 </c:pt>
@@ -421,6 +427,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,7 +527,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -656,10 +665,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.7211108344129716E-2"/>
-          <c:y val="0.15719682767711612"/>
-          <c:w val="0.90189257103831544"/>
-          <c:h val="0.69795987433844164"/>
+          <c:x val="6.6469816272965873E-2"/>
+          <c:y val="0.1585329969469732"/>
+          <c:w val="0.90297462817147855"/>
+          <c:h val="0.70099140836828866"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -670,11 +679,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>main!$F$5</c:f>
+              <c:f>main!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Post Lunch</c:v>
+                  <c:v>Post Breakfast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -682,7 +691,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -695,7 +704,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -708,10 +717,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$18:$A$32</c:f>
+              <c:f>main!$A$18:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>45475</c:v>
                 </c:pt>
@@ -756,57 +765,66 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$F$18:$F$32</c:f>
+              <c:f>main!$D$18:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.7</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.3</c:v>
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.0">
+                  <c:v>4.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -814,7 +832,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C9E1-4CB4-8319-D292F3021994}"/>
+              <c16:uniqueId val="{00000000-0131-442B-8E89-76AE3ED60F37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -827,11 +845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2137095568"/>
-        <c:axId val="2137095088"/>
+        <c:axId val="1922468256"/>
+        <c:axId val="1922465376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2137095568"/>
+        <c:axId val="1922468256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137095088"/>
+        <c:crossAx val="1922465376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -883,10 +901,10 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2137095088"/>
+        <c:axId val="1922465376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="16"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -935,7 +953,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137095568"/>
+        <c:crossAx val="1922468256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1068,9 +1086,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.7736989937087363E-2"/>
-          <c:y val="9.6396163858813333E-2"/>
+          <c:y val="8.8368207184494452E-2"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.76814376152965225"/>
+          <c:h val="0.77617171820397113"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1104,10 +1122,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1188,16 +1206,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$32</c:f>
+              <c:f>main!$C$6:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -1278,6 +1299,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1317,10 +1341,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1401,16 +1425,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$32</c:f>
+              <c:f>main!$E$6:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1491,6 +1518,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,10 +1560,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1614,16 +1644,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$32</c:f>
+              <c:f>main!$G$6:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -1701,6 +1734,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1740,10 +1776,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1824,16 +1860,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$32</c:f>
+              <c:f>main!$H$6:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -1902,6 +1941,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,10 +2271,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2313,16 +2355,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$32</c:f>
+              <c:f>main!$C$6:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -2403,6 +2448,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2690,10 +2738,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2774,16 +2822,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$32</c:f>
+              <c:f>main!$E$6:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -2864,6 +2915,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3101,9 +3155,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.6469816272965873E-2"/>
-          <c:y val="0.13834445466465026"/>
+          <c:y val="0.14033389447934172"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.75646067364363345"/>
+          <c:h val="0.74365458816269303"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3152,10 +3206,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3236,16 +3290,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$32</c:f>
+              <c:f>main!$G$6:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -3323,6 +3380,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3638,10 +3698,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3722,16 +3782,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$I$6:$I$32</c:f>
+              <c:f>main!$I$6:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
@@ -3775,6 +3838,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3836,10 +3902,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3920,16 +3986,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$J$6:$J$32</c:f>
+              <c:f>main!$J$6:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4009,6 +4078,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -4344,10 +4416,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4428,16 +4500,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$K$6:$K$32</c:f>
+              <c:f>main!$K$6:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4509,6 +4584,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4746,9 +4824,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.6469816272965873E-2"/>
-          <c:y val="0.14163437687197547"/>
+          <c:y val="0.1575590115889127"/>
           <c:w val="0.90297462817147855"/>
-          <c:h val="0.75133641654679184"/>
+          <c:h val="0.72552446841807883"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4800,10 +4878,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$32</c:f>
+              <c:f>main!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4884,16 +4962,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>45489</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45490</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$32</c:f>
+              <c:f>main!$H$6:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -4962,6 +5043,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5197,10 +5281,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.6304056132634293E-2"/>
-          <c:y val="0.15807068665648721"/>
-          <c:w val="0.90321658670471683"/>
-          <c:h val="0.71954027778191176"/>
+          <c:x val="6.7211108344129716E-2"/>
+          <c:y val="0.15719682767711612"/>
+          <c:w val="0.90189257103831544"/>
+          <c:h val="0.69795987433844164"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5211,11 +5295,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>main!$D$5</c:f>
+              <c:f>main!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Post Breakfast</c:v>
+                  <c:v>Post Lunch</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5223,7 +5307,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5236,7 +5320,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -5303,54 +5387,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$D$18:$D$32</c:f>
+              <c:f>main!$F$18:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.8</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.1</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.2</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0">
-                  <c:v>9.75</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.0">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.0">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.0">
-                  <c:v>8.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.0">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.0">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.0">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.0">
-                  <c:v>7.9</c:v>
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5358,7 +5442,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1FC8-49B1-A015-7B4FEEE1BF49}"/>
+              <c16:uniqueId val="{00000000-C9E1-4CB4-8319-D292F3021994}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5371,11 +5455,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1319217616"/>
-        <c:axId val="1319221456"/>
+        <c:axId val="2137095568"/>
+        <c:axId val="2137095088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1319217616"/>
+        <c:axId val="2137095568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5418,7 +5502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319221456"/>
+        <c:crossAx val="2137095088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5427,10 +5511,10 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1319221456"/>
+        <c:axId val="2137095088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5479,7 +5563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319217616"/>
+        <c:crossAx val="2137095568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11202,8 +11286,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>408565</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>128419</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11232,13 +11316,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>133912</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>150832</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>9301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11274,8 +11358,8 @@
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>459441</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>169431</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11340,13 +11424,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>130998</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>44824</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>171337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11375,22 +11459,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>431426</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12439</xdr:rowOff>
+      <xdr:colOff>416410</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>75864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>44824</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF16A46B-307B-D506-5C5D-DFEBCF2BB06F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC900005-D475-85C8-C9B2-2E60406442EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11411,22 +11495,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>416410</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>75864</xdr:rowOff>
+      <xdr:colOff>439238</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12791</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>44824</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>130661</xdr:rowOff>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>88991</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC900005-D475-85C8-C9B2-2E60406442EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6360F5-96FA-B1C8-FDBA-AFB8B7F0F2B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11448,11 +11532,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K32" totalsRowShown="0">
-  <autoFilter ref="A5:K32" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K33" totalsRowShown="0">
+  <autoFilter ref="A5:K33" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight"/>
+    <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E5B64DB2-CAD1-4DC4-923F-5F20775B475A}" name="Morning (07:15)"/>
     <tableColumn id="9" xr3:uid="{8610C2D9-DA3D-495E-A7DA-1A087E914E11}" name="Post Breakfast"/>
     <tableColumn id="4" xr3:uid="{00F66A78-6A41-4945-84A6-A1E12629EBFE}" name="Lunch (12:50)"/>
@@ -11784,24 +11868,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
-  <dimension ref="A1:AD52"/>
+  <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM21" sqref="AM21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="1.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -11834,49 +11918,49 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B63)</f>
-        <v>74.618518518518499</v>
+        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B64)</f>
+        <v>74.703571428571422</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" si="0"/>
-        <v>9.0740740740740744</v>
+        <v>8.9428571428571448</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" si="0"/>
-        <v>7.71</v>
+        <v>7.5218750000000005</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>11.714814814814813</v>
+        <v>11.546428571428569</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>9.1928571428571413</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>11.923076923076923</v>
+        <v>11.662962962962963</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>8.0260869565217394</v>
+        <v>7.875</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <f>MAX(B6:B70)</f>
-        <v>76.599999999999994</v>
+      <c r="B3" s="2">
+        <f>MAX(B6:B71)</f>
+        <v>77</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H3" si="1">MIN(C6:C70)</f>
+        <f t="shared" ref="C3:H3" si="1">MIN(C6:C71)</f>
         <v>5.2</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
@@ -11892,7 +11976,7 @@
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -11934,7 +12018,7 @@
       <c r="A6" s="1">
         <v>45463</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>72.400000000000006</v>
       </c>
       <c r="C6">
@@ -11954,7 +12038,7 @@
       <c r="A7" s="1">
         <v>45464</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>71.2</v>
       </c>
       <c r="C7">
@@ -11974,7 +12058,7 @@
       <c r="A8" s="1">
         <v>45465</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>73.400000000000006</v>
       </c>
       <c r="C8">
@@ -11997,7 +12081,7 @@
       <c r="A9" s="1">
         <v>45466</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>72.900000000000006</v>
       </c>
       <c r="C9">
@@ -12023,7 +12107,7 @@
       <c r="A10" s="1">
         <v>45467</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>73.5</v>
       </c>
       <c r="C10">
@@ -12049,7 +12133,7 @@
       <c r="A11" s="1">
         <v>45468</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>73</v>
       </c>
       <c r="C11">
@@ -12075,7 +12159,7 @@
       <c r="A12" s="1">
         <v>45469</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>73.7</v>
       </c>
       <c r="C12">
@@ -12101,7 +12185,7 @@
       <c r="A13" s="1">
         <v>45470</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>74</v>
       </c>
       <c r="C13">
@@ -12127,7 +12211,7 @@
       <c r="A14" s="1">
         <v>45471</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>74.5</v>
       </c>
       <c r="C14">
@@ -12153,7 +12237,7 @@
       <c r="A15" s="1">
         <v>45472</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>75.3</v>
       </c>
       <c r="C15">
@@ -12179,7 +12263,7 @@
       <c r="A16" s="1">
         <v>45473</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>75.099999999999994</v>
       </c>
       <c r="C16">
@@ -12205,7 +12289,7 @@
       <c r="A17" s="1">
         <v>45474</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>74.3</v>
       </c>
       <c r="C17">
@@ -12231,7 +12315,7 @@
       <c r="A18" s="1">
         <v>45475</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>74.7</v>
       </c>
       <c r="C18">
@@ -12266,7 +12350,7 @@
       <c r="A19" s="1">
         <v>45476</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>74.099999999999994</v>
       </c>
       <c r="C19">
@@ -12301,7 +12385,7 @@
       <c r="A20" s="1">
         <v>45477</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>74.7</v>
       </c>
       <c r="C20">
@@ -12336,7 +12420,7 @@
       <c r="A21" s="1">
         <v>45478</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>74.7</v>
       </c>
       <c r="C21">
@@ -12371,7 +12455,7 @@
       <c r="A22" s="1">
         <v>45479</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>75.599999999999994</v>
       </c>
       <c r="C22">
@@ -12407,7 +12491,7 @@
       <c r="A23" s="1">
         <v>45480</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>75.599999999999994</v>
       </c>
       <c r="C23">
@@ -12442,7 +12526,7 @@
       <c r="A24" s="1">
         <v>45481</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>75</v>
       </c>
       <c r="C24">
@@ -12477,7 +12561,7 @@
       <c r="A25" s="1">
         <v>45482</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>75.5</v>
       </c>
       <c r="C25">
@@ -12512,7 +12596,7 @@
       <c r="A26" s="1">
         <v>45483</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>75.8</v>
       </c>
       <c r="C26">
@@ -12547,7 +12631,7 @@
       <c r="A27" s="1">
         <v>45484</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>75.5</v>
       </c>
       <c r="C27">
@@ -12582,7 +12666,7 @@
       <c r="A28" s="1">
         <v>45485</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>75.599999999999994</v>
       </c>
       <c r="C28">
@@ -12617,7 +12701,7 @@
       <c r="A29" s="1">
         <v>45486</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>75.5</v>
       </c>
       <c r="C29">
@@ -12652,7 +12736,7 @@
       <c r="A30" s="1">
         <v>45487</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>76.3</v>
       </c>
       <c r="C30">
@@ -12687,7 +12771,7 @@
       <c r="A31" s="1">
         <v>45488</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>76.2</v>
       </c>
       <c r="C31">
@@ -12722,7 +12806,7 @@
       <c r="A32" s="1">
         <v>45489</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>76.599999999999994</v>
       </c>
       <c r="C32">
@@ -12734,20 +12818,55 @@
       <c r="E32">
         <v>5.5</v>
       </c>
+      <c r="F32">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G32">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H32">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="I32">
         <v>10</v>
       </c>
       <c r="J32">
         <v>10</v>
       </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45490</v>
+      </c>
+      <c r="B33" s="2">
+        <v>77</v>
+      </c>
+      <c r="C33">
+        <v>5.4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="30:30" x14ac:dyDescent="0.3">
-      <c r="AD52" t="s">
+    <row r="49" spans="30:30" x14ac:dyDescent="0.3">
+      <c r="AD49" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New data, fixed sidebar, made TODO
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="485" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF93448-2275-468D-9FD2-1F99F1F20828}"/>
+  <xr:revisionPtr revIDLastSave="497" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10171EA-D638-45B0-9902-71FC4B314247}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Weight</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Post Lunch</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -250,10 +253,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -337,16 +340,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$B$6:$B$33</c:f>
+              <c:f>main!$B$6:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>72.400000000000006</c:v>
                 </c:pt>
@@ -430,6 +436,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>77.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,7 +536,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1122,10 +1131,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1209,16 +1218,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$33</c:f>
+              <c:f>main!$C$6:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -1302,6 +1314,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1341,10 +1356,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1428,16 +1443,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$33</c:f>
+              <c:f>main!$E$6:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1560,10 +1578,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1647,16 +1665,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$33</c:f>
+              <c:f>main!$G$6:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -1779,10 +1800,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1866,16 +1887,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$33</c:f>
+              <c:f>main!$H$6:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -2277,10 +2301,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2364,16 +2388,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$33</c:f>
+              <c:f>main!$C$6:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -2457,6 +2484,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,10 +2774,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2831,16 +2861,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$33</c:f>
+              <c:f>main!$E$6:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -3212,10 +3245,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3299,16 +3332,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$33</c:f>
+              <c:f>main!$G$6:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -3707,10 +3743,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3794,16 +3830,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$I$6:$I$33</c:f>
+              <c:f>main!$I$6:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
@@ -3850,6 +3889,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3911,10 +3953,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3998,16 +4040,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$J$6:$J$33</c:f>
+              <c:f>main!$J$6:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4090,6 +4135,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -4425,10 +4473,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4512,16 +4560,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$K$6:$K$33</c:f>
+              <c:f>main!$K$6:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4596,6 +4647,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4887,10 +4941,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$33</c:f>
+              <c:f>main!$A$6:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4974,16 +5028,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>45490</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$33</c:f>
+              <c:f>main!$H$6:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -11545,8 +11602,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K33" totalsRowShown="0">
-  <autoFilter ref="A5:K33" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K34" totalsRowShown="0">
+  <autoFilter ref="A5:K34" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight" dataDxfId="0"/>
@@ -11884,21 +11941,21 @@
   <dimension ref="A1:AD49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="1.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -11931,31 +11988,31 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B64)</f>
-        <v>74.703571428571422</v>
+        <f>AVERAGE(B6:B65)</f>
+        <v>74.793103448275858</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" si="0"/>
-        <v>8.9428571428571448</v>
+        <f>AVERAGE(C6:C65)</f>
+        <v>8.7862068965517253</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
-        <v>7.5218750000000005</v>
+        <f>AVERAGE(D6:D65)</f>
+        <v>7.3441176470588241</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E6:E65)</f>
         <v>11.546428571428569</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F6:F65)</f>
         <v>9.1</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G6:G65)</f>
         <v>11.392857142857142</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H6:H65)</f>
         <v>7.8039999999999994</v>
       </c>
     </row>
@@ -11964,31 +12021,31 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <f>MAX(B6:B71)</f>
-        <v>77</v>
+        <f>MAX(B6:B72)</f>
+        <v>77.3</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H3" si="1">MIN(C6:C71)</f>
-        <v>5.2</v>
+        <f>MIN(C6:C72)</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
-        <v>4.7</v>
+        <f>MIN(D6:D72)</f>
+        <v>4.5</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f>MIN(E6:E72)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f>MIN(F6:F72)</f>
         <v>5.0999999999999996</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>MIN(G6:G72)</f>
         <v>4.0999999999999996</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
+        <f>MIN(H6:H72)</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -12359,7 +12416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45476</v>
       </c>
@@ -12394,7 +12451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45477</v>
       </c>
@@ -12850,7 +12907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45490</v>
       </c>
@@ -12881,9 +12938,35 @@
       <c r="J33">
         <v>10</v>
       </c>
+      <c r="K33">
+        <v>9</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H36" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45491</v>
+      </c>
+      <c r="B34" s="2">
+        <v>77.3</v>
+      </c>
+      <c r="C34">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I34">
+        <v>10</v>
+      </c>
+      <c r="J34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data and created the pie chart for porportion of readings
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="497" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10171EA-D638-45B0-9902-71FC4B314247}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC1DC4A9-2EFD-48A6-A8DC-3460E50479ED}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -1539,6 +1539,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2957,6 +2960,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11601,6 +11607,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K34" totalsRowShown="0">
   <autoFilter ref="A5:K34" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
@@ -11941,7 +11951,7 @@
   <dimension ref="A1:AD49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11988,31 +11998,31 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(B6:B65)</f>
+        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B65)</f>
         <v>74.793103448275858</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(C6:C65)</f>
+        <f t="shared" si="0"/>
         <v>8.7862068965517253</v>
       </c>
       <c r="D2" s="2">
-        <f>AVERAGE(D6:D65)</f>
+        <f t="shared" si="0"/>
         <v>7.3441176470588241</v>
       </c>
       <c r="E2" s="2">
-        <f>AVERAGE(E6:E65)</f>
-        <v>11.546428571428569</v>
+        <f t="shared" si="0"/>
+        <v>11.358620689655172</v>
       </c>
       <c r="F2" s="2">
-        <f>AVERAGE(F6:F65)</f>
+        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
       <c r="G2" s="2">
-        <f>AVERAGE(G6:G65)</f>
+        <f t="shared" si="0"/>
         <v>11.392857142857142</v>
       </c>
       <c r="H2" s="2">
-        <f>AVERAGE(H6:H65)</f>
+        <f t="shared" si="0"/>
         <v>7.8039999999999994</v>
       </c>
     </row>
@@ -12025,27 +12035,27 @@
         <v>77.3</v>
       </c>
       <c r="C3">
-        <f>MIN(C6:C72)</f>
+        <f t="shared" ref="C3:H3" si="1">MIN(C6:C72)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="D3">
-        <f>MIN(D6:D72)</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="E3">
-        <f>MIN(E6:E72)</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="F3">
-        <f>MIN(F6:F72)</f>
+        <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="G3">
-        <f>MIN(G6:G72)</f>
+        <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="H3">
-        <f>MIN(H6:H72)</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -12954,6 +12964,9 @@
       </c>
       <c r="D34" s="2">
         <v>4.5</v>
+      </c>
+      <c r="E34">
+        <v>6.1</v>
       </c>
       <c r="I34">
         <v>10</v>

</xml_diff>

<commit_message>
New data and fixed container sizing
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC1DC4A9-2EFD-48A6-A8DC-3460E50479ED}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F64361A2-0D67-4AA0-8BE0-09E86F01F1DD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -253,10 +253,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -343,16 +343,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$B$6:$B$34</c:f>
+              <c:f>main!$B$6:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>72.400000000000006</c:v>
                 </c:pt>
@@ -439,6 +442,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>77.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>76.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1131,10 +1137,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1221,16 +1227,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$34</c:f>
+              <c:f>main!$C$6:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -1317,6 +1326,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1356,10 +1368,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1446,16 +1458,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$34</c:f>
+              <c:f>main!$E$6:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1581,10 +1596,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1671,16 +1686,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$34</c:f>
+              <c:f>main!$G$6:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -1764,6 +1782,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,10 +1824,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1893,16 +1914,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$34</c:f>
+              <c:f>main!$H$6:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -1977,6 +2001,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,10 +2331,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2394,16 +2421,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$34</c:f>
+              <c:f>main!$C$6:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -2490,6 +2520,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2777,10 +2810,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2867,16 +2900,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$34</c:f>
+              <c:f>main!$E$6:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -3251,10 +3287,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3341,16 +3377,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$34</c:f>
+              <c:f>main!$G$6:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -3434,6 +3473,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3749,10 +3791,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3839,16 +3881,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$I$6:$I$34</c:f>
+              <c:f>main!$I$6:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
@@ -3898,6 +3943,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3959,10 +4007,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4049,16 +4097,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$J$6:$J$34</c:f>
+              <c:f>main!$J$6:$J$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4145,6 +4196,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4311,7 +4365,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4479,10 +4533,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4569,16 +4623,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$K$6:$K$34</c:f>
+              <c:f>main!$K$6:$K$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4655,6 +4712,9 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -4947,10 +5007,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$34</c:f>
+              <c:f>main!$A$6:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -5037,16 +5097,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45491</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$34</c:f>
+              <c:f>main!$H$6:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -5121,6 +5184,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11429,13 +11495,13 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>59841</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>134695</xdr:rowOff>
+      <xdr:rowOff>134694</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>459441</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11607,13 +11673,9 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K34" totalsRowShown="0">
-  <autoFilter ref="A5:K34" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K35" totalsRowShown="0">
+  <autoFilter ref="A5:K35" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight" dataDxfId="0"/>
@@ -11950,8 +12012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH47" sqref="AH47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11998,32 +12060,32 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B65)</f>
-        <v>74.793103448275858</v>
+        <f>AVERAGE(B6:B66)</f>
+        <v>74.86</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" si="0"/>
-        <v>8.7862068965517253</v>
+        <f>AVERAGE(C6:C66)</f>
+        <v>8.663333333333334</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6:D66)</f>
         <v>7.3441176470588241</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E6:E66)</f>
         <v>11.358620689655172</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
-        <v>9.1</v>
+        <f>AVERAGE(F6:F66)</f>
+        <v>9.0176470588235276</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
-        <v>11.392857142857142</v>
+        <f>AVERAGE(G6:G66)</f>
+        <v>11.248275862068965</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" si="0"/>
-        <v>7.8039999999999994</v>
+        <f>AVERAGE(H6:H66)</f>
+        <v>7.7999999999999989</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -12031,31 +12093,31 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <f>MAX(B6:B72)</f>
+        <f>MAX(B6:B73)</f>
         <v>77.3</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H3" si="1">MIN(C6:C72)</f>
+        <f>MIN(C6:C73)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
+        <f>MIN(D6:D73)</f>
         <v>4.5</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f>MIN(E6:E73)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f>MIN(F6:F73)</f>
         <v>5.0999999999999996</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>MIN(G6:G73)</f>
         <v>4.0999999999999996</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
+        <f>MIN(H6:H73)</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -12968,18 +13030,48 @@
       <c r="E34">
         <v>6.1</v>
       </c>
+      <c r="F34">
+        <v>7.7</v>
+      </c>
+      <c r="G34">
+        <v>7.2</v>
+      </c>
+      <c r="H34">
+        <v>7.7</v>
+      </c>
       <c r="I34">
         <v>10</v>
       </c>
       <c r="J34">
         <v>10</v>
       </c>
+      <c r="K34">
+        <v>9</v>
+      </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45492</v>
+      </c>
+      <c r="B35" s="2">
+        <v>76.8</v>
+      </c>
+      <c r="C35">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data, last update before deploying on Streamlit Cloud
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F64361A2-0D67-4AA0-8BE0-09E86F01F1DD}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49D7095-5173-4329-A0FA-D3C11F6A9B28}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -253,10 +253,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -346,16 +346,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$B$6:$B$35</c:f>
+              <c:f>main!$B$6:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>72.400000000000006</c:v>
                 </c:pt>
@@ -445,6 +448,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>76.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>77.099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,10 +1143,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1230,16 +1236,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$35</c:f>
+              <c:f>main!$C$6:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -1329,6 +1338,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1368,10 +1380,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1461,16 +1473,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$35</c:f>
+              <c:f>main!$E$6:$E$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1557,6 +1572,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1596,10 +1614,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1689,16 +1707,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$35</c:f>
+              <c:f>main!$G$6:$G$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -1785,6 +1806,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1824,10 +1848,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -1917,16 +1941,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$35</c:f>
+              <c:f>main!$H$6:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -2004,6 +2031,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,10 +2361,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2424,16 +2454,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$C$6:$C$35</c:f>
+              <c:f>main!$C$6:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>14.6</c:v>
                 </c:pt>
@@ -2523,6 +2556,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2810,10 +2846,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -2903,16 +2939,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$E$6:$E$35</c:f>
+              <c:f>main!$E$6:$E$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -2999,6 +3038,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3287,10 +3329,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3380,16 +3422,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$G$6:$G$35</c:f>
+              <c:f>main!$G$6:$G$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>16.5</c:v>
                 </c:pt>
@@ -3476,6 +3521,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3791,10 +3839,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -3884,16 +3932,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$I$6:$I$35</c:f>
+              <c:f>main!$I$6:$I$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
@@ -3946,6 +3997,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -4007,10 +4061,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4100,16 +4154,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$J$6:$J$35</c:f>
+              <c:f>main!$J$6:$J$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4198,6 +4255,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4533,10 +4593,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -4626,16 +4686,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$K$6:$K$35</c:f>
+              <c:f>main!$K$6:$K$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4716,6 +4779,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5007,10 +5073,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>main!$A$6:$A$35</c:f>
+              <c:f>main!$A$6:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>45463</c:v>
                 </c:pt>
@@ -5100,16 +5166,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>main!$H$6:$H$35</c:f>
+              <c:f>main!$H$6:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="3">
                   <c:v>14.2</c:v>
                 </c:pt>
@@ -5187,6 +5256,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11673,9 +11745,13 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K35" totalsRowShown="0">
-  <autoFilter ref="A5:K35" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K36" totalsRowShown="0">
+  <autoFilter ref="A5:K36" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F3B13052-68BF-4C97-BCA9-A385B988D19D}" name="Date " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{75CE39A0-3FAC-4324-B899-84EFA5722702}" name="Weight" dataDxfId="0"/>
@@ -12012,8 +12088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH47" sqref="AH47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12060,32 +12136,32 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(B6:B66)</f>
-        <v>74.86</v>
+        <f t="shared" ref="B2:H2" si="0">AVERAGE(B6:B67)</f>
+        <v>74.932258064516134</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(C6:C66)</f>
-        <v>8.663333333333334</v>
+        <f t="shared" si="0"/>
+        <v>8.5354838709677434</v>
       </c>
       <c r="D2" s="2">
-        <f>AVERAGE(D6:D66)</f>
-        <v>7.3441176470588241</v>
+        <f t="shared" si="0"/>
+        <v>7.0131578947368434</v>
       </c>
       <c r="E2" s="2">
-        <f>AVERAGE(E6:E66)</f>
-        <v>11.358620689655172</v>
+        <f t="shared" si="0"/>
+        <v>11.156666666666666</v>
       </c>
       <c r="F2" s="2">
-        <f>AVERAGE(F6:F66)</f>
-        <v>9.0176470588235276</v>
+        <f t="shared" si="0"/>
+        <v>9.0555555555555536</v>
       </c>
       <c r="G2" s="2">
-        <f>AVERAGE(G6:G66)</f>
-        <v>11.248275862068965</v>
+        <f t="shared" si="0"/>
+        <v>11.036666666666665</v>
       </c>
       <c r="H2" s="2">
-        <f>AVERAGE(H6:H66)</f>
-        <v>7.7999999999999989</v>
+        <f t="shared" si="0"/>
+        <v>7.7518518518518515</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -12093,31 +12169,31 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <f>MAX(B6:B73)</f>
+        <f>MAX(B6:B74)</f>
         <v>77.3</v>
       </c>
       <c r="C3">
-        <f>MIN(C6:C73)</f>
+        <f t="shared" ref="C3:H3" si="1">MIN(C6:C74)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="D3">
-        <f>MIN(D6:D73)</f>
-        <v>4.5</v>
+        <f t="shared" si="1"/>
+        <v>3.9</v>
       </c>
       <c r="E3">
-        <f>MIN(E6:E73)</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="F3">
-        <f>MIN(F6:F73)</f>
+        <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="G3">
-        <f>MIN(G6:G73)</f>
+        <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="H3">
-        <f>MIN(H6:H73)</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -13059,19 +13135,56 @@
       <c r="C35">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E35">
+        <v>5.3</v>
+      </c>
+      <c r="F35">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G35">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H35">
+        <v>6.5</v>
+      </c>
       <c r="I35">
         <v>10</v>
       </c>
       <c r="J35">
         <v>8</v>
       </c>
+      <c r="K35">
+        <v>10</v>
+      </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45493</v>
+      </c>
+      <c r="B36" s="2">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="C36">
+        <v>4.7</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>14</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data, graphs, and images.
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49D7095-5173-4329-A0FA-D3C11F6A9B28}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80BDD965-3920-4CAB-877C-52EDF54FFA94}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -1576,6 +1576,9 @@
                 <c:pt idx="29">
                   <c:v>5.3</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1809,6 +1812,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3042,6 +3048,9 @@
                 <c:pt idx="29">
                   <c:v>5.3</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3524,6 +3533,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5496,9 +5508,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.7211108344129716E-2"/>
-          <c:y val="0.15719682767711612"/>
+          <c:y val="0.19417824593771857"/>
           <c:w val="0.90189257103831544"/>
-          <c:h val="0.69795987433844164"/>
+          <c:h val="0.66837480206187605"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -11745,10 +11757,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}" name="Table2" displayName="Table2" ref="A5:K36" totalsRowShown="0">
   <autoFilter ref="A5:K36" xr:uid="{98229571-E852-4D72-AD88-420739E80AA6}"/>
@@ -12088,8 +12096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12149,15 +12157,15 @@
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>11.156666666666666</v>
+        <v>10.92258064516129</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>9.0555555555555536</v>
+        <v>8.9421052631578934</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>11.036666666666665</v>
+        <v>10.835483870967741</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
@@ -12182,7 +12190,7 @@
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
       <c r="F3">
         <f t="shared" si="1"/>
@@ -13172,6 +13180,15 @@
       </c>
       <c r="D36" s="2">
         <v>3.9</v>
+      </c>
+      <c r="E36">
+        <v>3.9</v>
+      </c>
+      <c r="F36">
+        <v>6.9</v>
+      </c>
+      <c r="G36">
+        <v>4.8</v>
       </c>
       <c r="I36">
         <v>10</v>

</xml_diff>

<commit_message>
Added data, updated graphs, fixed last issues before deploying
</commit_message>
<xml_diff>
--- a/DiabetesTracker.xlsx
+++ b/DiabetesTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heiway-my.sharepoint.com/personal/evertc02_heiway_net/Documents/Documents/streamlit-and-analytics/my_flask_app/DiabetesTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80BDD965-3920-4CAB-877C-52EDF54FFA94}"/>
+  <xr:revisionPtr revIDLastSave="529" documentId="13_ncr:1_{9E831668-67EE-495A-A50A-64C123260486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D9F5806-861F-4618-8F89-8C6FD4484308}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5319E4B5-F908-47AC-8797-7A3F1E090568}"/>
   </bookViews>
@@ -2040,6 +2040,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5271,6 +5274,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12096,8 +12102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B1A06E-97E0-492A-AFA3-9B50FA5CE61B}">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12169,7 +12175,7 @@
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>7.7518518518518515</v>
+        <v>7.7392857142857139</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -13189,6 +13195,9 @@
       </c>
       <c r="G36">
         <v>4.8</v>
+      </c>
+      <c r="H36">
+        <v>7.4</v>
       </c>
       <c r="I36">
         <v>10</v>

</xml_diff>